<commit_message>
Changes ppt and excel
</commit_message>
<xml_diff>
--- a/docs/cs543_report.xlsx
+++ b/docs/cs543_report.xlsx
@@ -100,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -109,6 +109,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -428,7 +431,7 @@
   <dimension ref="B3:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -486,22 +489,22 @@
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>57.2</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>68.2</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <v>60.9</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="4">
         <v>63.9</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="4">
         <v>57.9</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="4">
         <v>60.5</v>
       </c>
       <c r="I5" s="1">
@@ -512,22 +515,22 @@
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>52.8</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>79.400000000000006</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="4">
         <v>61.8</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="4">
         <v>67.099999999999994</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="4">
         <v>54.1</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="4">
         <v>58.8</v>
       </c>
       <c r="I6" s="1">
@@ -538,22 +541,22 @@
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <v>65.5</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>28.8</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="4">
         <v>36.6</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="4">
         <v>58.6</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="4">
         <v>50</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="4">
         <v>52.3</v>
       </c>
       <c r="I7" s="1">
@@ -564,22 +567,22 @@
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>49.3</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>44.5</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>45.5</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="4">
         <v>45.1</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="4">
         <v>48.5</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="4">
         <v>46.5</v>
       </c>
       <c r="I8" s="1">
@@ -629,22 +632,22 @@
       <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="4">
         <v>59</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="4">
         <v>88.3</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="4">
         <v>69.400000000000006</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="4">
         <v>63.9</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="4">
         <v>28.3</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="4">
         <v>38.5</v>
       </c>
       <c r="I15" s="1">
@@ -655,22 +658,22 @@
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="4">
         <v>53.7</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="4">
         <v>98.5</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="4">
         <v>68.099999999999994</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="4">
         <v>75.599999999999994</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="4">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="4">
         <v>15.8</v>
       </c>
       <c r="I16" s="1">
@@ -681,22 +684,22 @@
       <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="4">
         <v>53.1</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="4">
         <v>95.4</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="4">
         <v>67.099999999999994</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="4">
         <v>71.2</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="4">
         <v>5.2</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="4">
         <v>9.6</v>
       </c>
       <c r="I17" s="1">
@@ -707,22 +710,22 @@
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="4">
         <v>58.2</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="4">
         <v>61.3</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="4">
         <v>58.4</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="4">
         <v>36.1</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="4">
         <v>32.1</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="4">
         <v>33.5</v>
       </c>
       <c r="I18" s="1">

</xml_diff>